<commit_message>
Updated With Webdriver manager
</commit_message>
<xml_diff>
--- a/WSS05.Project.SeleniumExpert/src/test/resources/testData.xlsx
+++ b/WSS05.Project.SeleniumExpert/src/test/resources/testData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>TC_Login_001</t>
   </si>
@@ -82,16 +83,36 @@
   </si>
   <si>
     <t>TC_Login_021</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>!@#@$%</t>
+  </si>
+  <si>
+    <t>123khjgf</t>
+  </si>
+  <si>
+    <t>hsd skdhf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,13 +135,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,4 +562,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1">
+        <v>12345</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>